<commit_message>
Template Change and Ratecard Code added
Template Change and Ratecard Code added
</commit_message>
<xml_diff>
--- a/bins/VMO2 CS TEMPLATE.xlsx
+++ b/bins/VMO2 CS TEMPLATE.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lsammon\Desktop\Python\quote generator\bins\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lsammon\Documents\GitHub\quotegenerator\bins\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9D0BCBD-1F93-4CBD-8279-330C4CB6CD1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9322376C-D344-47FB-9B56-A96F86960455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33000" yWindow="4200" windowWidth="17280" windowHeight="8970" xr2:uid="{45130684-8006-4796-B42E-75FFD46064F9}"/>
+    <workbookView xWindow="1380" yWindow="2436" windowWidth="17280" windowHeight="8976" xr2:uid="{45130684-8006-4796-B42E-75FFD46064F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -800,41 +800,26 @@
     <xf numFmtId="49" fontId="13" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -863,26 +848,41 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="3" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="3" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
@@ -1324,43 +1324,43 @@
       <c r="A4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="121"/>
-      <c r="C4" s="122"/>
+      <c r="B4" s="100"/>
+      <c r="C4" s="101"/>
     </row>
     <row r="5" spans="1:10" ht="12" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="121"/>
-      <c r="C5" s="122"/>
+      <c r="B5" s="100"/>
+      <c r="C5" s="101"/>
     </row>
     <row r="6" spans="1:10" ht="12" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="123"/>
-      <c r="C6" s="122"/>
+      <c r="B6" s="102"/>
+      <c r="C6" s="101"/>
     </row>
     <row r="7" spans="1:10" ht="12" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B7" s="123"/>
-      <c r="C7" s="125"/>
+      <c r="B7" s="102"/>
+      <c r="C7" s="104"/>
     </row>
     <row r="8" spans="1:10" ht="12" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="121"/>
-      <c r="C8" s="122"/>
+      <c r="B8" s="100"/>
+      <c r="C8" s="101"/>
     </row>
     <row r="9" spans="1:10" ht="12" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="124"/>
-      <c r="C9" s="122"/>
+      <c r="B9" s="103"/>
+      <c r="C9" s="101"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:10" ht="12" x14ac:dyDescent="0.25">
@@ -1370,86 +1370,86 @@
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="119" t="s">
+      <c r="G11" s="98" t="s">
         <v>2</v>
       </c>
-      <c r="H11" s="119"/>
-      <c r="I11" s="119" t="s">
+      <c r="H11" s="98"/>
+      <c r="I11" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="J11" s="120"/>
+      <c r="J11" s="99"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G12" s="108"/>
-      <c r="H12" s="108"/>
-      <c r="I12" s="108"/>
-      <c r="J12" s="108"/>
+      <c r="G12" s="114"/>
+      <c r="H12" s="114"/>
+      <c r="I12" s="114"/>
+      <c r="J12" s="114"/>
     </row>
     <row r="13" spans="1:10" ht="12" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G13" s="109"/>
-      <c r="H13" s="109"/>
-      <c r="I13" s="109"/>
-      <c r="J13" s="109"/>
+      <c r="G13" s="115"/>
+      <c r="H13" s="115"/>
+      <c r="I13" s="115"/>
+      <c r="J13" s="115"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G14" s="107"/>
-      <c r="H14" s="107"/>
-      <c r="I14" s="107"/>
-      <c r="J14" s="107"/>
+      <c r="G14" s="116"/>
+      <c r="H14" s="116"/>
+      <c r="I14" s="116"/>
+      <c r="J14" s="116"/>
     </row>
     <row r="15" spans="1:10" ht="12" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G15" s="107">
+      <c r="G15" s="116">
         <f>SUM(Ratecard!F5:F7)</f>
         <v>0</v>
       </c>
-      <c r="H15" s="107"/>
-      <c r="I15" s="107">
+      <c r="H15" s="116"/>
+      <c r="I15" s="116">
         <f>Ratecard!N5</f>
         <v>0</v>
       </c>
-      <c r="J15" s="107"/>
+      <c r="J15" s="116"/>
     </row>
     <row r="16" spans="1:10" ht="12" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G16" s="107">
+      <c r="G16" s="116">
         <f>Ratecard!F8</f>
         <v>0</v>
       </c>
-      <c r="H16" s="107"/>
-      <c r="I16" s="107">
+      <c r="H16" s="116"/>
+      <c r="I16" s="116">
         <f>Ratecard!N59</f>
         <v>0</v>
       </c>
-      <c r="J16" s="107"/>
+      <c r="J16" s="116"/>
     </row>
     <row r="17" spans="1:10" ht="12" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G17" s="107">
+      <c r="G17" s="116">
         <f>SUM(Ratecard!F9:F11)</f>
         <v>0</v>
       </c>
-      <c r="H17" s="107"/>
-      <c r="I17" s="107">
+      <c r="H17" s="116"/>
+      <c r="I17" s="116">
         <f>Ratecard!N79</f>
         <v>0</v>
       </c>
-      <c r="J17" s="107"/>
+      <c r="J17" s="116"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G18" s="106"/>
-      <c r="H18" s="106"/>
-      <c r="I18" s="106"/>
-      <c r="J18" s="106"/>
+      <c r="G18" s="125"/>
+      <c r="H18" s="125"/>
+      <c r="I18" s="125"/>
+      <c r="J18" s="125"/>
     </row>
     <row r="19" spans="1:10" ht="12" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
@@ -1460,16 +1460,16 @@
       <c r="D19" s="13"/>
       <c r="E19" s="13"/>
       <c r="F19" s="14"/>
-      <c r="G19" s="98">
+      <c r="G19" s="117">
         <f>SUM(G14:G18)</f>
         <v>0</v>
       </c>
-      <c r="H19" s="99"/>
-      <c r="I19" s="98">
+      <c r="H19" s="118"/>
+      <c r="I19" s="117">
         <f>SUM(I15:J17)</f>
         <v>0</v>
       </c>
-      <c r="J19" s="99"/>
+      <c r="J19" s="118"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2"/>
     <row r="21" spans="1:10" ht="12" x14ac:dyDescent="0.25">
@@ -1482,10 +1482,10 @@
       <c r="E21" s="8"/>
     </row>
     <row r="22" spans="1:10" ht="12" x14ac:dyDescent="0.25">
-      <c r="A22" s="100"/>
-      <c r="B22" s="101"/>
-      <c r="C22" s="101"/>
-      <c r="D22" s="102"/>
+      <c r="A22" s="119"/>
+      <c r="B22" s="120"/>
+      <c r="C22" s="120"/>
+      <c r="D22" s="121"/>
       <c r="E22" s="8"/>
       <c r="F22" s="17" t="s">
         <v>6</v>
@@ -1498,17 +1498,17 @@
       <c r="J22" s="9"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" s="100"/>
-      <c r="B23" s="101"/>
-      <c r="C23" s="101"/>
-      <c r="D23" s="102"/>
+      <c r="A23" s="119"/>
+      <c r="B23" s="120"/>
+      <c r="C23" s="120"/>
+      <c r="D23" s="121"/>
       <c r="E23" s="8"/>
     </row>
     <row r="24" spans="1:10" ht="12" x14ac:dyDescent="0.25">
-      <c r="A24" s="103"/>
-      <c r="B24" s="104"/>
-      <c r="C24" s="104"/>
-      <c r="D24" s="105"/>
+      <c r="A24" s="122"/>
+      <c r="B24" s="123"/>
+      <c r="C24" s="123"/>
+      <c r="D24" s="124"/>
       <c r="E24" s="8"/>
       <c r="F24" s="17" t="s">
         <v>8</v>
@@ -1543,58 +1543,58 @@
       <c r="J26" s="15"/>
     </row>
     <row r="27" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="110"/>
-      <c r="B27" s="111"/>
-      <c r="C27" s="111"/>
-      <c r="D27" s="112"/>
+      <c r="A27" s="105"/>
+      <c r="B27" s="106"/>
+      <c r="C27" s="106"/>
+      <c r="D27" s="107"/>
     </row>
     <row r="28" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="113"/>
-      <c r="B28" s="114"/>
-      <c r="C28" s="114"/>
-      <c r="D28" s="115"/>
+      <c r="A28" s="108"/>
+      <c r="B28" s="109"/>
+      <c r="C28" s="109"/>
+      <c r="D28" s="110"/>
     </row>
     <row r="29" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="113"/>
-      <c r="B29" s="114"/>
-      <c r="C29" s="114"/>
-      <c r="D29" s="115"/>
+      <c r="A29" s="108"/>
+      <c r="B29" s="109"/>
+      <c r="C29" s="109"/>
+      <c r="D29" s="110"/>
     </row>
     <row r="30" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="113"/>
-      <c r="B30" s="114"/>
-      <c r="C30" s="114"/>
-      <c r="D30" s="115"/>
+      <c r="A30" s="108"/>
+      <c r="B30" s="109"/>
+      <c r="C30" s="109"/>
+      <c r="D30" s="110"/>
     </row>
     <row r="31" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="113"/>
-      <c r="B31" s="114"/>
-      <c r="C31" s="114"/>
-      <c r="D31" s="115"/>
+      <c r="A31" s="108"/>
+      <c r="B31" s="109"/>
+      <c r="C31" s="109"/>
+      <c r="D31" s="110"/>
     </row>
     <row r="32" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="113"/>
-      <c r="B32" s="114"/>
-      <c r="C32" s="114"/>
-      <c r="D32" s="115"/>
+      <c r="A32" s="108"/>
+      <c r="B32" s="109"/>
+      <c r="C32" s="109"/>
+      <c r="D32" s="110"/>
     </row>
     <row r="33" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="113"/>
-      <c r="B33" s="114"/>
-      <c r="C33" s="114"/>
-      <c r="D33" s="115"/>
+      <c r="A33" s="108"/>
+      <c r="B33" s="109"/>
+      <c r="C33" s="109"/>
+      <c r="D33" s="110"/>
     </row>
     <row r="34" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="113"/>
-      <c r="B34" s="114"/>
-      <c r="C34" s="114"/>
-      <c r="D34" s="115"/>
+      <c r="A34" s="108"/>
+      <c r="B34" s="109"/>
+      <c r="C34" s="109"/>
+      <c r="D34" s="110"/>
     </row>
     <row r="35" spans="1:10" ht="12" x14ac:dyDescent="0.25">
-      <c r="A35" s="113"/>
-      <c r="B35" s="114"/>
-      <c r="C35" s="114"/>
-      <c r="D35" s="115"/>
+      <c r="A35" s="108"/>
+      <c r="B35" s="109"/>
+      <c r="C35" s="109"/>
+      <c r="D35" s="110"/>
       <c r="F35" s="17" t="s">
         <v>6</v>
       </c>
@@ -1606,16 +1606,16 @@
       <c r="J35" s="9"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36" s="113"/>
-      <c r="B36" s="114"/>
-      <c r="C36" s="114"/>
-      <c r="D36" s="115"/>
+      <c r="A36" s="108"/>
+      <c r="B36" s="109"/>
+      <c r="C36" s="109"/>
+      <c r="D36" s="110"/>
     </row>
     <row r="37" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="113"/>
-      <c r="B37" s="114"/>
-      <c r="C37" s="114"/>
-      <c r="D37" s="115"/>
+      <c r="A37" s="108"/>
+      <c r="B37" s="109"/>
+      <c r="C37" s="109"/>
+      <c r="D37" s="110"/>
       <c r="F37" s="17" t="s">
         <v>38</v>
       </c>
@@ -1625,10 +1625,10 @@
       <c r="J37" s="9"/>
     </row>
     <row r="38" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="113"/>
-      <c r="B38" s="114"/>
-      <c r="C38" s="114"/>
-      <c r="D38" s="115"/>
+      <c r="A38" s="108"/>
+      <c r="B38" s="109"/>
+      <c r="C38" s="109"/>
+      <c r="D38" s="110"/>
       <c r="F38" s="17" t="s">
         <v>9</v>
       </c>
@@ -1638,46 +1638,46 @@
       <c r="J38" s="9"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A39" s="113"/>
-      <c r="B39" s="114"/>
-      <c r="C39" s="114"/>
-      <c r="D39" s="115"/>
+      <c r="A39" s="108"/>
+      <c r="B39" s="109"/>
+      <c r="C39" s="109"/>
+      <c r="D39" s="110"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A40" s="113"/>
-      <c r="B40" s="114"/>
-      <c r="C40" s="114"/>
-      <c r="D40" s="115"/>
+      <c r="A40" s="108"/>
+      <c r="B40" s="109"/>
+      <c r="C40" s="109"/>
+      <c r="D40" s="110"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A41" s="113"/>
-      <c r="B41" s="114"/>
-      <c r="C41" s="114"/>
-      <c r="D41" s="115"/>
+      <c r="A41" s="108"/>
+      <c r="B41" s="109"/>
+      <c r="C41" s="109"/>
+      <c r="D41" s="110"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A42" s="113"/>
-      <c r="B42" s="114"/>
-      <c r="C42" s="114"/>
-      <c r="D42" s="115"/>
+      <c r="A42" s="108"/>
+      <c r="B42" s="109"/>
+      <c r="C42" s="109"/>
+      <c r="D42" s="110"/>
     </row>
     <row r="43" spans="1:10" ht="108.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="113"/>
-      <c r="B43" s="114"/>
-      <c r="C43" s="114"/>
-      <c r="D43" s="115"/>
+      <c r="A43" s="108"/>
+      <c r="B43" s="109"/>
+      <c r="C43" s="109"/>
+      <c r="D43" s="110"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A44" s="113"/>
-      <c r="B44" s="114"/>
-      <c r="C44" s="114"/>
-      <c r="D44" s="115"/>
+      <c r="A44" s="108"/>
+      <c r="B44" s="109"/>
+      <c r="C44" s="109"/>
+      <c r="D44" s="110"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A45" s="116"/>
-      <c r="B45" s="117"/>
-      <c r="C45" s="117"/>
-      <c r="D45" s="118"/>
+      <c r="A45" s="111"/>
+      <c r="B45" s="112"/>
+      <c r="C45" s="112"/>
+      <c r="D45" s="113"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2"/>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2"/>
@@ -1697,6 +1697,24 @@
     <row r="61" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="A22:D24"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="A27:D45"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G17:H17"/>
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="I11:J11"/>
     <mergeCell ref="B4:C4"/>
@@ -1705,24 +1723,6 @@
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B7:C7"/>
-    <mergeCell ref="A27:D45"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="A22:D24"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1735,7 +1735,7 @@
   <dimension ref="A1:S2090"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -1903,7 +1903,9 @@
       <c r="D6" s="57">
         <v>428.34</v>
       </c>
-      <c r="E6" s="38"/>
+      <c r="E6" s="38">
+        <v>0</v>
+      </c>
       <c r="F6" s="89">
         <f t="shared" ref="F6:F11" si="0">D6*E6</f>
         <v>0</v>
@@ -1933,7 +1935,9 @@
       <c r="D7" s="57">
         <v>203.19</v>
       </c>
-      <c r="E7" s="38"/>
+      <c r="E7" s="38">
+        <v>0</v>
+      </c>
       <c r="F7" s="89">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1993,7 +1997,9 @@
       <c r="D9" s="57">
         <v>126.3</v>
       </c>
-      <c r="E9" s="38"/>
+      <c r="E9" s="38">
+        <v>0</v>
+      </c>
       <c r="F9" s="89">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2023,7 +2029,9 @@
       <c r="D10" s="57">
         <v>203.19</v>
       </c>
-      <c r="E10" s="38"/>
+      <c r="E10" s="38">
+        <v>0</v>
+      </c>
       <c r="F10" s="89">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2053,7 +2061,9 @@
       <c r="D11" s="57">
         <v>727.07</v>
       </c>
-      <c r="E11" s="38"/>
+      <c r="E11" s="38">
+        <v>0</v>
+      </c>
       <c r="F11" s="89">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -14884,12 +14894,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003AB5751ECABA6749998EF74675425B7B" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="70ed28ac003b6d379fa35ade6abc2863">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="39a94dcf-b6e2-4f89-b70c-f1c9b6ab0e61" xmlns:ns4="62ff2926-d3aa-4d63-a80f-1987d6b279cc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7e138214fb60f7ac65bb94e3793bb0af" ns3:_="" ns4:_="">
     <xsd:import namespace="39a94dcf-b6e2-4f89-b70c-f1c9b6ab0e61"/>
@@ -15112,6 +15116,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -15122,15 +15132,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F138C2C4-D118-4DE3-AAEA-5BBC3FF040F7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E7C5A98-C3A1-4BF8-8017-645861449BF9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15149,6 +15150,15 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F138C2C4-D118-4DE3-AAEA-5BBC3FF040F7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2921983E-6AF9-412A-AD58-3980A2719A16}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
New filename and hide button 2
</commit_message>
<xml_diff>
--- a/bins/VMO2 CS TEMPLATE.xlsx
+++ b/bins/VMO2 CS TEMPLATE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lsammon\Desktop\Python\quote generator\bins\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2AB8616-C76C-41AB-BB1F-03FC1E6C493E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16CB3850-262F-4231-B72B-034B73BBCD56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{45130684-8006-4796-B42E-75FFD46064F9}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{45130684-8006-4796-B42E-75FFD46064F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -800,26 +800,41 @@
     <xf numFmtId="49" fontId="13" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="3" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="3" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -848,41 +863,26 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
@@ -1292,7 +1292,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F69775E9-4FEB-4A52-A827-5ECFC7C93FAC}">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B8" sqref="B8:C8"/>
     </sheetView>
   </sheetViews>
@@ -1324,45 +1324,45 @@
       <c r="A4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="100"/>
-      <c r="C4" s="101"/>
+      <c r="B4" s="121"/>
+      <c r="C4" s="122"/>
     </row>
     <row r="5" spans="1:10" ht="12" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="100"/>
-      <c r="C5" s="101"/>
+      <c r="B5" s="121"/>
+      <c r="C5" s="122"/>
     </row>
     <row r="6" spans="1:10" ht="12" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="102"/>
-      <c r="C6" s="101"/>
+      <c r="B6" s="123"/>
+      <c r="C6" s="122"/>
     </row>
     <row r="7" spans="1:10" ht="12" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B7" s="102"/>
-      <c r="C7" s="104"/>
+      <c r="B7" s="123"/>
+      <c r="C7" s="125"/>
     </row>
     <row r="8" spans="1:10" ht="12" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="100" t="s">
+      <c r="B8" s="121" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="101"/>
+      <c r="C8" s="122"/>
     </row>
     <row r="9" spans="1:10" ht="12" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="103"/>
-      <c r="C9" s="101"/>
+      <c r="B9" s="124"/>
+      <c r="C9" s="122"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:10" ht="12" x14ac:dyDescent="0.25">
@@ -1372,86 +1372,86 @@
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="98" t="s">
+      <c r="G11" s="119" t="s">
         <v>2</v>
       </c>
-      <c r="H11" s="98"/>
-      <c r="I11" s="98" t="s">
+      <c r="H11" s="119"/>
+      <c r="I11" s="119" t="s">
         <v>3</v>
       </c>
-      <c r="J11" s="99"/>
+      <c r="J11" s="120"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G12" s="114"/>
-      <c r="H12" s="114"/>
-      <c r="I12" s="114"/>
-      <c r="J12" s="114"/>
+      <c r="G12" s="108"/>
+      <c r="H12" s="108"/>
+      <c r="I12" s="108"/>
+      <c r="J12" s="108"/>
     </row>
     <row r="13" spans="1:10" ht="12" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G13" s="115"/>
-      <c r="H13" s="115"/>
-      <c r="I13" s="115"/>
-      <c r="J13" s="115"/>
+      <c r="G13" s="109"/>
+      <c r="H13" s="109"/>
+      <c r="I13" s="109"/>
+      <c r="J13" s="109"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G14" s="116"/>
-      <c r="H14" s="116"/>
-      <c r="I14" s="116"/>
-      <c r="J14" s="116"/>
+      <c r="G14" s="107"/>
+      <c r="H14" s="107"/>
+      <c r="I14" s="107"/>
+      <c r="J14" s="107"/>
     </row>
     <row r="15" spans="1:10" ht="12" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G15" s="116">
+      <c r="G15" s="107">
         <f>SUM(Ratecard!F5:F7)</f>
         <v>1586.45</v>
       </c>
-      <c r="H15" s="116"/>
-      <c r="I15" s="116">
+      <c r="H15" s="107"/>
+      <c r="I15" s="107">
         <f>Ratecard!N5</f>
         <v>0</v>
       </c>
-      <c r="J15" s="116"/>
+      <c r="J15" s="107"/>
     </row>
     <row r="16" spans="1:10" ht="12" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G16" s="116">
+      <c r="G16" s="107">
         <f>Ratecard!F8</f>
         <v>0</v>
       </c>
-      <c r="H16" s="116"/>
-      <c r="I16" s="116">
+      <c r="H16" s="107"/>
+      <c r="I16" s="107">
         <f>Ratecard!N59</f>
         <v>0</v>
       </c>
-      <c r="J16" s="116"/>
+      <c r="J16" s="107"/>
     </row>
     <row r="17" spans="1:10" ht="12" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G17" s="116">
+      <c r="G17" s="107">
         <f>SUM(Ratecard!F9:F11)</f>
         <v>0</v>
       </c>
-      <c r="H17" s="116"/>
-      <c r="I17" s="116">
+      <c r="H17" s="107"/>
+      <c r="I17" s="107">
         <f>Ratecard!N79</f>
         <v>0</v>
       </c>
-      <c r="J17" s="116"/>
+      <c r="J17" s="107"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G18" s="125"/>
-      <c r="H18" s="125"/>
-      <c r="I18" s="125"/>
-      <c r="J18" s="125"/>
+      <c r="G18" s="106"/>
+      <c r="H18" s="106"/>
+      <c r="I18" s="106"/>
+      <c r="J18" s="106"/>
     </row>
     <row r="19" spans="1:10" ht="12" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
@@ -1462,16 +1462,16 @@
       <c r="D19" s="13"/>
       <c r="E19" s="13"/>
       <c r="F19" s="14"/>
-      <c r="G19" s="117">
+      <c r="G19" s="98">
         <f>SUM(G14:G18)</f>
         <v>1586.45</v>
       </c>
-      <c r="H19" s="118"/>
-      <c r="I19" s="117">
+      <c r="H19" s="99"/>
+      <c r="I19" s="98">
         <f>SUM(I15:J17)</f>
         <v>0</v>
       </c>
-      <c r="J19" s="118"/>
+      <c r="J19" s="99"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2"/>
     <row r="21" spans="1:10" ht="12" x14ac:dyDescent="0.25">
@@ -1484,10 +1484,10 @@
       <c r="E21" s="8"/>
     </row>
     <row r="22" spans="1:10" ht="12" x14ac:dyDescent="0.25">
-      <c r="A22" s="119"/>
-      <c r="B22" s="120"/>
-      <c r="C22" s="120"/>
-      <c r="D22" s="121"/>
+      <c r="A22" s="100"/>
+      <c r="B22" s="101"/>
+      <c r="C22" s="101"/>
+      <c r="D22" s="102"/>
       <c r="E22" s="8"/>
       <c r="F22" s="17" t="s">
         <v>6</v>
@@ -1500,17 +1500,17 @@
       <c r="J22" s="9"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" s="119"/>
-      <c r="B23" s="120"/>
-      <c r="C23" s="120"/>
-      <c r="D23" s="121"/>
+      <c r="A23" s="100"/>
+      <c r="B23" s="101"/>
+      <c r="C23" s="101"/>
+      <c r="D23" s="102"/>
       <c r="E23" s="8"/>
     </row>
     <row r="24" spans="1:10" ht="12" x14ac:dyDescent="0.25">
-      <c r="A24" s="122"/>
-      <c r="B24" s="123"/>
-      <c r="C24" s="123"/>
-      <c r="D24" s="124"/>
+      <c r="A24" s="103"/>
+      <c r="B24" s="104"/>
+      <c r="C24" s="104"/>
+      <c r="D24" s="105"/>
       <c r="E24" s="8"/>
       <c r="F24" s="17" t="s">
         <v>8</v>
@@ -1545,58 +1545,58 @@
       <c r="J26" s="15"/>
     </row>
     <row r="27" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="105"/>
-      <c r="B27" s="106"/>
-      <c r="C27" s="106"/>
-      <c r="D27" s="107"/>
+      <c r="A27" s="110"/>
+      <c r="B27" s="111"/>
+      <c r="C27" s="111"/>
+      <c r="D27" s="112"/>
     </row>
     <row r="28" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="108"/>
-      <c r="B28" s="109"/>
-      <c r="C28" s="109"/>
-      <c r="D28" s="110"/>
+      <c r="A28" s="113"/>
+      <c r="B28" s="114"/>
+      <c r="C28" s="114"/>
+      <c r="D28" s="115"/>
     </row>
     <row r="29" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="108"/>
-      <c r="B29" s="109"/>
-      <c r="C29" s="109"/>
-      <c r="D29" s="110"/>
+      <c r="A29" s="113"/>
+      <c r="B29" s="114"/>
+      <c r="C29" s="114"/>
+      <c r="D29" s="115"/>
     </row>
     <row r="30" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="108"/>
-      <c r="B30" s="109"/>
-      <c r="C30" s="109"/>
-      <c r="D30" s="110"/>
+      <c r="A30" s="113"/>
+      <c r="B30" s="114"/>
+      <c r="C30" s="114"/>
+      <c r="D30" s="115"/>
     </row>
     <row r="31" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="108"/>
-      <c r="B31" s="109"/>
-      <c r="C31" s="109"/>
-      <c r="D31" s="110"/>
+      <c r="A31" s="113"/>
+      <c r="B31" s="114"/>
+      <c r="C31" s="114"/>
+      <c r="D31" s="115"/>
     </row>
     <row r="32" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="108"/>
-      <c r="B32" s="109"/>
-      <c r="C32" s="109"/>
-      <c r="D32" s="110"/>
+      <c r="A32" s="113"/>
+      <c r="B32" s="114"/>
+      <c r="C32" s="114"/>
+      <c r="D32" s="115"/>
     </row>
     <row r="33" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="108"/>
-      <c r="B33" s="109"/>
-      <c r="C33" s="109"/>
-      <c r="D33" s="110"/>
+      <c r="A33" s="113"/>
+      <c r="B33" s="114"/>
+      <c r="C33" s="114"/>
+      <c r="D33" s="115"/>
     </row>
     <row r="34" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="108"/>
-      <c r="B34" s="109"/>
-      <c r="C34" s="109"/>
-      <c r="D34" s="110"/>
+      <c r="A34" s="113"/>
+      <c r="B34" s="114"/>
+      <c r="C34" s="114"/>
+      <c r="D34" s="115"/>
     </row>
     <row r="35" spans="1:10" ht="12" x14ac:dyDescent="0.25">
-      <c r="A35" s="108"/>
-      <c r="B35" s="109"/>
-      <c r="C35" s="109"/>
-      <c r="D35" s="110"/>
+      <c r="A35" s="113"/>
+      <c r="B35" s="114"/>
+      <c r="C35" s="114"/>
+      <c r="D35" s="115"/>
       <c r="F35" s="17" t="s">
         <v>6</v>
       </c>
@@ -1608,16 +1608,16 @@
       <c r="J35" s="9"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36" s="108"/>
-      <c r="B36" s="109"/>
-      <c r="C36" s="109"/>
-      <c r="D36" s="110"/>
+      <c r="A36" s="113"/>
+      <c r="B36" s="114"/>
+      <c r="C36" s="114"/>
+      <c r="D36" s="115"/>
     </row>
     <row r="37" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="108"/>
-      <c r="B37" s="109"/>
-      <c r="C37" s="109"/>
-      <c r="D37" s="110"/>
+      <c r="A37" s="113"/>
+      <c r="B37" s="114"/>
+      <c r="C37" s="114"/>
+      <c r="D37" s="115"/>
       <c r="F37" s="17" t="s">
         <v>38</v>
       </c>
@@ -1627,10 +1627,10 @@
       <c r="J37" s="9"/>
     </row>
     <row r="38" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="108"/>
-      <c r="B38" s="109"/>
-      <c r="C38" s="109"/>
-      <c r="D38" s="110"/>
+      <c r="A38" s="113"/>
+      <c r="B38" s="114"/>
+      <c r="C38" s="114"/>
+      <c r="D38" s="115"/>
       <c r="F38" s="17" t="s">
         <v>9</v>
       </c>
@@ -1640,46 +1640,46 @@
       <c r="J38" s="9"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A39" s="108"/>
-      <c r="B39" s="109"/>
-      <c r="C39" s="109"/>
-      <c r="D39" s="110"/>
+      <c r="A39" s="113"/>
+      <c r="B39" s="114"/>
+      <c r="C39" s="114"/>
+      <c r="D39" s="115"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A40" s="108"/>
-      <c r="B40" s="109"/>
-      <c r="C40" s="109"/>
-      <c r="D40" s="110"/>
+      <c r="A40" s="113"/>
+      <c r="B40" s="114"/>
+      <c r="C40" s="114"/>
+      <c r="D40" s="115"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A41" s="108"/>
-      <c r="B41" s="109"/>
-      <c r="C41" s="109"/>
-      <c r="D41" s="110"/>
+      <c r="A41" s="113"/>
+      <c r="B41" s="114"/>
+      <c r="C41" s="114"/>
+      <c r="D41" s="115"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A42" s="108"/>
-      <c r="B42" s="109"/>
-      <c r="C42" s="109"/>
-      <c r="D42" s="110"/>
+      <c r="A42" s="113"/>
+      <c r="B42" s="114"/>
+      <c r="C42" s="114"/>
+      <c r="D42" s="115"/>
     </row>
     <row r="43" spans="1:10" ht="108.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="108"/>
-      <c r="B43" s="109"/>
-      <c r="C43" s="109"/>
-      <c r="D43" s="110"/>
+      <c r="A43" s="113"/>
+      <c r="B43" s="114"/>
+      <c r="C43" s="114"/>
+      <c r="D43" s="115"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A44" s="108"/>
-      <c r="B44" s="109"/>
-      <c r="C44" s="109"/>
-      <c r="D44" s="110"/>
+      <c r="A44" s="113"/>
+      <c r="B44" s="114"/>
+      <c r="C44" s="114"/>
+      <c r="D44" s="115"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A45" s="111"/>
-      <c r="B45" s="112"/>
-      <c r="C45" s="112"/>
-      <c r="D45" s="113"/>
+      <c r="A45" s="116"/>
+      <c r="B45" s="117"/>
+      <c r="C45" s="117"/>
+      <c r="D45" s="118"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2"/>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2"/>
@@ -1699,24 +1699,6 @@
     <row r="61" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="A22:D24"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="A27:D45"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G17:H17"/>
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="I11:J11"/>
     <mergeCell ref="B4:C4"/>
@@ -1725,6 +1707,24 @@
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B7:C7"/>
+    <mergeCell ref="A27:D45"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="A22:D24"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1736,7 +1736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C205F163-B46B-49EE-AC67-253FDBCA891D}">
   <dimension ref="A1:S2090"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -14896,6 +14896,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003AB5751ECABA6749998EF74675425B7B" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="70ed28ac003b6d379fa35ade6abc2863">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="39a94dcf-b6e2-4f89-b70c-f1c9b6ab0e61" xmlns:ns4="62ff2926-d3aa-4d63-a80f-1987d6b279cc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7e138214fb60f7ac65bb94e3793bb0af" ns3:_="" ns4:_="">
     <xsd:import namespace="39a94dcf-b6e2-4f89-b70c-f1c9b6ab0e61"/>
@@ -15118,22 +15133,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2921983E-6AF9-412A-AD58-3980A2719A16}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F138C2C4-D118-4DE3-AAEA-5BBC3FF040F7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E7C5A98-C3A1-4BF8-8017-645861449BF9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15150,21 +15167,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F138C2C4-D118-4DE3-AAEA-5BBC3FF040F7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2921983E-6AF9-412A-AD58-3980A2719A16}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Version 2.0 Source Code
</commit_message>
<xml_diff>
--- a/bins/VMO2 CS TEMPLATE.xlsx
+++ b/bins/VMO2 CS TEMPLATE.xlsx
@@ -1,29 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lsammon\Desktop\Python\quote generator\bins\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lsammon\Desktop\Python\database testing\bins\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16CB3850-262F-4231-B72B-034B73BBCD56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{70C2A5BA-E681-4C51-AABE-65157F3BDC2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{45130684-8006-4796-B42E-75FFD46064F9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Summary" sheetId="2" r:id="rId1"/>
-    <sheet name="Ratecard" sheetId="3" r:id="rId2"/>
+    <sheet name="Summary" sheetId="1" r:id="rId1"/>
+    <sheet name="Ratecard" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Ratecard!$B$4:$O$372</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -32,6 +29,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -41,13 +39,28 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
   <si>
+    <t>NET COVERAGE SOLUTIONS  - VM02 2025</t>
+  </si>
+  <si>
+    <t>VM02 REF:</t>
+  </si>
+  <si>
+    <t>SITE NAME:</t>
+  </si>
+  <si>
+    <t>SITE ADDRESS:</t>
+  </si>
+  <si>
+    <t>POSTCODE:</t>
+  </si>
+  <si>
     <t>SUBMISSION TYPE</t>
   </si>
   <si>
-    <t>SUBMISSION DATE</t>
+    <t>Contract Sum</t>
   </si>
   <si>
-    <t>Contract Sum</t>
+    <t>SUBMISSION DATE</t>
   </si>
   <si>
     <t>Final Account</t>
@@ -56,7 +69,19 @@
     <t>Contract Sums</t>
   </si>
   <si>
+    <t>Decom Works</t>
+  </si>
+  <si>
+    <t>Symology Works</t>
+  </si>
+  <si>
+    <t>Access Equipment</t>
+  </si>
+  <si>
     <t>Total Site Cost</t>
+  </si>
+  <si>
+    <t>Document Used:</t>
   </si>
   <si>
     <t>Signed</t>
@@ -74,13 +99,13 @@
     <t>Exclusions / Notes:</t>
   </si>
   <si>
+    <t>For and on behalf of Virgin Media O2</t>
+  </si>
+  <si>
     <t>Item</t>
   </si>
   <si>
     <t>Description</t>
-  </si>
-  <si>
-    <t>C.Sum Qty</t>
   </si>
   <si>
     <t>Unit</t>
@@ -89,10 +114,19 @@
     <t>Rate</t>
   </si>
   <si>
+    <t>C.Sum Qty</t>
+  </si>
+  <si>
     <t>C.Sum Total</t>
   </si>
   <si>
     <t>NET Comments</t>
+  </si>
+  <si>
+    <t>VM02 / MCC Comments</t>
+  </si>
+  <si>
+    <t>Contract Sum totals</t>
   </si>
   <si>
     <t>F.Acc Qty</t>
@@ -101,22 +135,28 @@
     <t>F.AccTotal</t>
   </si>
   <si>
-    <t>item</t>
+    <t>Final Account Totals</t>
   </si>
   <si>
-    <t>SITE ADDRESS:</t>
-  </si>
-  <si>
-    <t>VM02 REF:</t>
-  </si>
-  <si>
-    <t>SITE NAME:</t>
+    <t>Change from Tender?</t>
   </si>
   <si>
     <t>Rate affected by geographical weightings defined in section 15?</t>
   </si>
   <si>
     <t>Relevant to London Microcell</t>
+  </si>
+  <si>
+    <t>14.02</t>
+  </si>
+  <si>
+    <t>Decommission a microcell solution as defined in section 2.6 of the main RFP requirements. To include the removal of up to 4 external antennas.</t>
+  </si>
+  <si>
+    <t>Split decom labour (Decommision of Antennas on separate date to internal equipment)</t>
+  </si>
+  <si>
+    <t>Out of hours uplift for Decommission labour</t>
   </si>
   <si>
     <t>Percentage uplift for Symology including EToN, TM Deployment, MEWP licenses and parking bay suspensions, chapter 8 barriers &amp; signage. A minimum of 2 competitive quotes to be provided with the Contract Sum to demonstrate good value</t>
@@ -131,55 +171,13 @@
     <t>Cherry picker (Hire costs per day including transport to and from site). Up to 25m in height</t>
   </si>
   <si>
-    <t>Split decom labour (Decommision of Antennas on separate date to internal equipment)</t>
-  </si>
-  <si>
-    <t>Out of hours uplift for Decommission labour</t>
-  </si>
-  <si>
-    <t>VM02 / MCC Comments</t>
-  </si>
-  <si>
-    <t>Change from Tender?</t>
-  </si>
-  <si>
-    <t>Contract Sum totals</t>
-  </si>
-  <si>
-    <t>Final Account Totals</t>
-  </si>
-  <si>
     <t>Blank to enable Variation to be added</t>
   </si>
   <si>
-    <t>Insert new variations above this line</t>
+    <t>item</t>
   </si>
   <si>
-    <t>For and on behalf of Virgin Media O2</t>
-  </si>
-  <si>
-    <t>Document Used:</t>
-  </si>
-  <si>
-    <t>NET COVERAGE SOLUTIONS  - VM02 2025</t>
-  </si>
-  <si>
-    <t>Decommission a microcell solution as defined in section 2.6 of the main RFP requirements. To include the removal of up to 4 external antennas.</t>
-  </si>
-  <si>
-    <t>14.02</t>
-  </si>
-  <si>
-    <t>Decom Works</t>
-  </si>
-  <si>
-    <t>Symology Works</t>
-  </si>
-  <si>
-    <t>Access Equipment</t>
-  </si>
-  <si>
-    <t>POSTCODE:</t>
+    <t>Insert new variations above this line</t>
   </si>
 </sst>
 </file>
@@ -190,8 +188,8 @@
     <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="&quot;£&quot;#,##0.00"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -353,7 +351,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -524,22 +522,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -595,7 +606,7 @@
     <xf numFmtId="44" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="44" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -626,7 +637,7 @@
     <xf numFmtId="2" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -647,7 +658,7 @@
     <xf numFmtId="49" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -663,13 +674,13 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -681,7 +692,7 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="13" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -699,13 +710,13 @@
     <xf numFmtId="49" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="11" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="11" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="11" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -717,7 +728,7 @@
     <xf numFmtId="49" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="8" fontId="13" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -800,103 +811,65 @@
     <xf numFmtId="49" fontId="13" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="44" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="3" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="2" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="12">
-    <cellStyle name="Comma 2" xfId="9" xr:uid="{DC071084-2586-4FEE-A2E3-5B21CC197544}"/>
-    <cellStyle name="Comma 2 2" xfId="10" xr:uid="{914464D5-29AC-4AFE-9C74-F0FD6205D2F0}"/>
-    <cellStyle name="Comma 2 3" xfId="11" xr:uid="{81A2F7CE-FEC5-4B8E-B86B-7BAE30868710}"/>
+    <cellStyle name="Comma 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Comma 2 2" xfId="10" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Comma 2 3" xfId="11" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
-    <cellStyle name="Currency 2" xfId="3" xr:uid="{864E0DC0-DEB6-4DDB-9095-C20E455E48EE}"/>
-    <cellStyle name="Currency 3" xfId="4" xr:uid="{680A1F0F-09C2-4E07-9543-BAAA403A6B4A}"/>
+    <cellStyle name="Currency 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Currency 3" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="7" xr:uid="{1183260A-1F38-4C8F-98BF-EB0A3D3249C7}"/>
-    <cellStyle name="Normal 3" xfId="6" xr:uid="{21EAE9FB-22EC-44B8-9F8A-1F22F3CCE41F}"/>
-    <cellStyle name="Normal 4" xfId="5" xr:uid="{CF0E2B5A-2107-4E74-A6E4-BF5FF7CB6D12}"/>
-    <cellStyle name="Normal 5" xfId="8" xr:uid="{2C5240BF-EBFA-4CCB-B687-741CBC3D980D}"/>
+    <cellStyle name="Normal 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Normal 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 4" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 5" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="3">
@@ -958,7 +931,7 @@
         <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38204ACB-E5D3-4437-89EB-2493BBDA24E3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -967,13 +940,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -986,6 +953,9 @@
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1289,250 +1259,248 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F69775E9-4FEB-4A52-A827-5ECFC7C93FAC}">
-  <dimension ref="A1:K61"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:C8"/>
+      <selection activeCell="A22" sqref="A22:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="11.4" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.77734375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.21875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="12.5546875" style="2" customWidth="1"/>
-    <col min="4" max="5" width="9.21875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="12.21875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11.77734375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="12.21875" style="2" customWidth="1"/>
+    <col min="4" max="5" width="9.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" style="2" customWidth="1"/>
     <col min="9" max="9" width="12.44140625" style="2" customWidth="1"/>
     <col min="10" max="10" width="12.5546875" style="2" customWidth="1"/>
-    <col min="11" max="11" width="9.21875" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="9.21875" style="2" hidden="1"/>
+    <col min="11" max="11" width="9.33203125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" style="2" hidden="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.33203125" style="2" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="12" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:10" ht="12" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="121"/>
-      <c r="C4" s="122"/>
-    </row>
-    <row r="5" spans="1:10" ht="12" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="121"/>
-      <c r="C5" s="122"/>
-    </row>
-    <row r="6" spans="1:10" ht="12" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="123"/>
-      <c r="C6" s="122"/>
-    </row>
-    <row r="7" spans="1:10" ht="12" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B7" s="123"/>
-      <c r="C7" s="125"/>
-    </row>
-    <row r="8" spans="1:10" ht="12" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="121" t="s">
+    </row>
+    <row r="2" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+    </row>
+    <row r="4" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="98"/>
+      <c r="C4" s="99"/>
+    </row>
+    <row r="5" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="122"/>
-    </row>
-    <row r="9" spans="1:10" ht="12" x14ac:dyDescent="0.25">
+      <c r="B5" s="98"/>
+      <c r="C5" s="99"/>
+    </row>
+    <row r="6" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="98"/>
+      <c r="C6" s="99"/>
+    </row>
+    <row r="7" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="104"/>
+      <c r="C7" s="99"/>
+    </row>
+    <row r="8" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="98" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="99"/>
+    </row>
+    <row r="9" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
-      <c r="B9" s="124"/>
-      <c r="C9" s="122"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:10" ht="12" x14ac:dyDescent="0.25">
+      <c r="B9" s="115"/>
+      <c r="C9" s="99"/>
+    </row>
+    <row r="11" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="119" t="s">
-        <v>2</v>
+      <c r="G11" s="118" t="s">
+        <v>6</v>
       </c>
       <c r="H11" s="119"/>
-      <c r="I11" s="119" t="s">
-        <v>3</v>
+      <c r="I11" s="105" t="s">
+        <v>8</v>
       </c>
-      <c r="J11" s="120"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G12" s="108"/>
-      <c r="H12" s="108"/>
-      <c r="I12" s="108"/>
-      <c r="J12" s="108"/>
-    </row>
-    <row r="13" spans="1:10" ht="12" x14ac:dyDescent="0.25">
+      <c r="J11" s="99"/>
+    </row>
+    <row r="12" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="G12" s="106"/>
+      <c r="H12" s="107"/>
+      <c r="I12" s="106"/>
+      <c r="J12" s="107"/>
+    </row>
+    <row r="13" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
-      <c r="G13" s="109"/>
-      <c r="H13" s="109"/>
-      <c r="I13" s="109"/>
-      <c r="J13" s="109"/>
+      <c r="G13" s="103"/>
+      <c r="H13" s="101"/>
+      <c r="I13" s="103"/>
+      <c r="J13" s="101"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G14" s="107"/>
-      <c r="H14" s="107"/>
-      <c r="I14" s="107"/>
-      <c r="J14" s="107"/>
-    </row>
-    <row r="15" spans="1:10" ht="12" x14ac:dyDescent="0.25">
+      <c r="G14" s="100"/>
+      <c r="H14" s="101"/>
+      <c r="I14" s="100"/>
+      <c r="J14" s="101"/>
+    </row>
+    <row r="15" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>43</v>
+        <v>10</v>
       </c>
-      <c r="G15" s="107">
+      <c r="G15" s="100">
         <f>SUM(Ratecard!F5:F7)</f>
-        <v>1586.45</v>
-      </c>
-      <c r="H15" s="107"/>
-      <c r="I15" s="107">
-        <f>Ratecard!N5</f>
         <v>0</v>
       </c>
-      <c r="J15" s="107"/>
-    </row>
-    <row r="16" spans="1:10" ht="12" x14ac:dyDescent="0.25">
+      <c r="H15" s="101"/>
+      <c r="I15" s="100">
+        <f>SUM(Ratecard!M5:M7)</f>
+        <v>0</v>
+      </c>
+      <c r="J15" s="101"/>
+    </row>
+    <row r="16" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
-      <c r="G16" s="107">
+      <c r="G16" s="100">
         <f>Ratecard!F8</f>
         <v>0</v>
       </c>
-      <c r="H16" s="107"/>
-      <c r="I16" s="107">
-        <f>Ratecard!N59</f>
+      <c r="H16" s="101"/>
+      <c r="I16" s="100">
+        <f>Ratecard!M8</f>
         <v>0</v>
       </c>
-      <c r="J16" s="107"/>
-    </row>
-    <row r="17" spans="1:10" ht="12" x14ac:dyDescent="0.25">
+      <c r="J16" s="101"/>
+    </row>
+    <row r="17" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
-      <c r="G17" s="107">
+      <c r="G17" s="100">
         <f>SUM(Ratecard!F9:F11)</f>
         <v>0</v>
       </c>
-      <c r="H17" s="107"/>
-      <c r="I17" s="107">
-        <f>Ratecard!N79</f>
+      <c r="H17" s="101"/>
+      <c r="I17" s="100">
+        <f>SUM(Ratecard!M9:M11)</f>
         <v>0</v>
       </c>
-      <c r="J17" s="107"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G18" s="106"/>
-      <c r="H18" s="106"/>
-      <c r="I18" s="106"/>
-      <c r="J18" s="106"/>
-    </row>
-    <row r="19" spans="1:10" ht="12" x14ac:dyDescent="0.25">
+      <c r="J17" s="101"/>
+    </row>
+    <row r="18" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="G18" s="117"/>
+      <c r="H18" s="113"/>
+      <c r="I18" s="117"/>
+      <c r="J18" s="113"/>
+    </row>
+    <row r="19" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="16" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B19" s="13"/>
       <c r="C19" s="13"/>
       <c r="D19" s="13"/>
       <c r="E19" s="13"/>
       <c r="F19" s="14"/>
-      <c r="G19" s="98">
+      <c r="G19" s="102">
         <f>SUM(G14:G18)</f>
-        <v>1586.45</v>
+        <v>0</v>
       </c>
       <c r="H19" s="99"/>
-      <c r="I19" s="98">
+      <c r="I19" s="102">
         <f>SUM(I15:J17)</f>
         <v>0</v>
       </c>
       <c r="J19" s="99"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="1:10" ht="12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="8"/>
     </row>
-    <row r="22" spans="1:10" ht="12" x14ac:dyDescent="0.25">
-      <c r="A22" s="100"/>
+    <row r="22" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="116"/>
       <c r="B22" s="101"/>
       <c r="C22" s="101"/>
-      <c r="D22" s="102"/>
+      <c r="D22" s="111"/>
       <c r="E22" s="8"/>
       <c r="F22" s="17" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="G22" s="9"/>
       <c r="H22" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" s="100"/>
+      <c r="A23" s="110"/>
       <c r="B23" s="101"/>
       <c r="C23" s="101"/>
-      <c r="D23" s="102"/>
+      <c r="D23" s="111"/>
       <c r="E23" s="8"/>
     </row>
-    <row r="24" spans="1:10" ht="12" x14ac:dyDescent="0.25">
-      <c r="A24" s="103"/>
-      <c r="B24" s="104"/>
-      <c r="C24" s="104"/>
-      <c r="D24" s="105"/>
+    <row r="24" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="112"/>
+      <c r="B24" s="113"/>
+      <c r="C24" s="113"/>
+      <c r="D24" s="114"/>
       <c r="E24" s="8"/>
       <c r="F24" s="17" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
       <c r="I24" s="9"/>
       <c r="J24" s="9"/>
     </row>
-    <row r="25" spans="1:10" ht="12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D25" s="13"/>
       <c r="F25" s="17" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
       <c r="I25" s="9"/>
       <c r="J25" s="9"/>
     </row>
-    <row r="26" spans="1:10" ht="12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
@@ -1545,81 +1513,81 @@
       <c r="J26" s="15"/>
     </row>
     <row r="27" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="110"/>
-      <c r="B27" s="111"/>
-      <c r="C27" s="111"/>
-      <c r="D27" s="112"/>
+      <c r="A27" s="108"/>
+      <c r="B27" s="107"/>
+      <c r="C27" s="107"/>
+      <c r="D27" s="109"/>
     </row>
     <row r="28" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="113"/>
-      <c r="B28" s="114"/>
-      <c r="C28" s="114"/>
-      <c r="D28" s="115"/>
+      <c r="A28" s="110"/>
+      <c r="B28" s="101"/>
+      <c r="C28" s="101"/>
+      <c r="D28" s="111"/>
     </row>
     <row r="29" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="113"/>
-      <c r="B29" s="114"/>
-      <c r="C29" s="114"/>
-      <c r="D29" s="115"/>
+      <c r="A29" s="110"/>
+      <c r="B29" s="101"/>
+      <c r="C29" s="101"/>
+      <c r="D29" s="111"/>
     </row>
     <row r="30" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="113"/>
-      <c r="B30" s="114"/>
-      <c r="C30" s="114"/>
-      <c r="D30" s="115"/>
+      <c r="A30" s="110"/>
+      <c r="B30" s="101"/>
+      <c r="C30" s="101"/>
+      <c r="D30" s="111"/>
     </row>
     <row r="31" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="113"/>
-      <c r="B31" s="114"/>
-      <c r="C31" s="114"/>
-      <c r="D31" s="115"/>
+      <c r="A31" s="110"/>
+      <c r="B31" s="101"/>
+      <c r="C31" s="101"/>
+      <c r="D31" s="111"/>
     </row>
     <row r="32" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="113"/>
-      <c r="B32" s="114"/>
-      <c r="C32" s="114"/>
-      <c r="D32" s="115"/>
+      <c r="A32" s="110"/>
+      <c r="B32" s="101"/>
+      <c r="C32" s="101"/>
+      <c r="D32" s="111"/>
     </row>
     <row r="33" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="113"/>
-      <c r="B33" s="114"/>
-      <c r="C33" s="114"/>
-      <c r="D33" s="115"/>
+      <c r="A33" s="110"/>
+      <c r="B33" s="101"/>
+      <c r="C33" s="101"/>
+      <c r="D33" s="111"/>
     </row>
     <row r="34" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="113"/>
-      <c r="B34" s="114"/>
-      <c r="C34" s="114"/>
-      <c r="D34" s="115"/>
-    </row>
-    <row r="35" spans="1:10" ht="12" x14ac:dyDescent="0.25">
-      <c r="A35" s="113"/>
-      <c r="B35" s="114"/>
-      <c r="C35" s="114"/>
-      <c r="D35" s="115"/>
+      <c r="A34" s="110"/>
+      <c r="B34" s="101"/>
+      <c r="C34" s="101"/>
+      <c r="D34" s="111"/>
+    </row>
+    <row r="35" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="110"/>
+      <c r="B35" s="101"/>
+      <c r="C35" s="101"/>
+      <c r="D35" s="111"/>
       <c r="F35" s="17" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="G35" s="9"/>
       <c r="H35" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="I35" s="9"/>
       <c r="J35" s="9"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36" s="113"/>
-      <c r="B36" s="114"/>
-      <c r="C36" s="114"/>
-      <c r="D36" s="115"/>
+      <c r="A36" s="110"/>
+      <c r="B36" s="101"/>
+      <c r="C36" s="101"/>
+      <c r="D36" s="111"/>
     </row>
     <row r="37" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="113"/>
-      <c r="B37" s="114"/>
-      <c r="C37" s="114"/>
-      <c r="D37" s="115"/>
+      <c r="A37" s="110"/>
+      <c r="B37" s="101"/>
+      <c r="C37" s="101"/>
+      <c r="D37" s="111"/>
       <c r="F37" s="17" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="G37" s="9"/>
       <c r="H37" s="9"/>
@@ -1627,12 +1595,12 @@
       <c r="J37" s="9"/>
     </row>
     <row r="38" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="113"/>
-      <c r="B38" s="114"/>
-      <c r="C38" s="114"/>
-      <c r="D38" s="115"/>
+      <c r="A38" s="110"/>
+      <c r="B38" s="101"/>
+      <c r="C38" s="101"/>
+      <c r="D38" s="111"/>
       <c r="F38" s="17" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="G38" s="9"/>
       <c r="H38" s="9"/>
@@ -1640,127 +1608,111 @@
       <c r="J38" s="9"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A39" s="113"/>
-      <c r="B39" s="114"/>
-      <c r="C39" s="114"/>
-      <c r="D39" s="115"/>
+      <c r="A39" s="110"/>
+      <c r="B39" s="101"/>
+      <c r="C39" s="101"/>
+      <c r="D39" s="111"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A40" s="113"/>
-      <c r="B40" s="114"/>
-      <c r="C40" s="114"/>
-      <c r="D40" s="115"/>
+      <c r="A40" s="110"/>
+      <c r="B40" s="101"/>
+      <c r="C40" s="101"/>
+      <c r="D40" s="111"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A41" s="113"/>
-      <c r="B41" s="114"/>
-      <c r="C41" s="114"/>
-      <c r="D41" s="115"/>
+      <c r="A41" s="110"/>
+      <c r="B41" s="101"/>
+      <c r="C41" s="101"/>
+      <c r="D41" s="111"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A42" s="113"/>
-      <c r="B42" s="114"/>
-      <c r="C42" s="114"/>
-      <c r="D42" s="115"/>
+      <c r="A42" s="110"/>
+      <c r="B42" s="101"/>
+      <c r="C42" s="101"/>
+      <c r="D42" s="111"/>
     </row>
     <row r="43" spans="1:10" ht="108.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="113"/>
-      <c r="B43" s="114"/>
-      <c r="C43" s="114"/>
-      <c r="D43" s="115"/>
+      <c r="A43" s="110"/>
+      <c r="B43" s="101"/>
+      <c r="C43" s="101"/>
+      <c r="D43" s="111"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A44" s="113"/>
-      <c r="B44" s="114"/>
-      <c r="C44" s="114"/>
-      <c r="D44" s="115"/>
+      <c r="A44" s="110"/>
+      <c r="B44" s="101"/>
+      <c r="C44" s="101"/>
+      <c r="D44" s="111"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A45" s="116"/>
-      <c r="B45" s="117"/>
-      <c r="C45" s="117"/>
-      <c r="D45" s="118"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2"/>
-    <row r="49" x14ac:dyDescent="0.2"/>
-    <row r="50" x14ac:dyDescent="0.2"/>
-    <row r="51" x14ac:dyDescent="0.2"/>
-    <row r="52" x14ac:dyDescent="0.2"/>
-    <row r="53" x14ac:dyDescent="0.2"/>
-    <row r="54" x14ac:dyDescent="0.2"/>
-    <row r="55" x14ac:dyDescent="0.2"/>
-    <row r="56" x14ac:dyDescent="0.2"/>
-    <row r="57" x14ac:dyDescent="0.2"/>
-    <row r="58" x14ac:dyDescent="0.2"/>
-    <row r="59" x14ac:dyDescent="0.2"/>
-    <row r="60" x14ac:dyDescent="0.2"/>
-    <row r="61" x14ac:dyDescent="0.2"/>
+      <c r="A45" s="112"/>
+      <c r="B45" s="113"/>
+      <c r="C45" s="113"/>
+      <c r="D45" s="114"/>
+    </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="A27:D45"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="I14:J14"/>
     <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="A27:D45"/>
-    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="A22:D24"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="G19:H19"/>
     <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="A22:D24"/>
-    <mergeCell ref="G19:H19"/>
     <mergeCell ref="G18:H18"/>
     <mergeCell ref="I18:J18"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="I12:J12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C205F163-B46B-49EE-AC67-253FDBCA891D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S2090"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.44140625" style="19" customWidth="1"/>
     <col min="2" max="2" width="51" style="11" customWidth="1"/>
-    <col min="3" max="3" width="7.77734375" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" style="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.44140625" style="29" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.21875" style="92" customWidth="1"/>
-    <col min="6" max="6" width="11.21875" style="87" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" style="92" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" style="87" customWidth="1"/>
     <col min="7" max="8" width="33.5546875" style="32" customWidth="1"/>
-    <col min="9" max="9" width="13.21875" style="87" customWidth="1"/>
-    <col min="10" max="10" width="6.21875" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" style="87" customWidth="1"/>
+    <col min="10" max="10" width="6.33203125" style="12" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.44140625" style="29" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.21875" style="92" customWidth="1"/>
-    <col min="13" max="13" width="11.21875" style="87" customWidth="1"/>
-    <col min="14" max="14" width="25.21875" style="32" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="11.33203125" style="92" customWidth="1"/>
+    <col min="13" max="13" width="11.33203125" style="87" customWidth="1"/>
+    <col min="14" max="14" width="25.33203125" style="32" hidden="1" customWidth="1"/>
     <col min="15" max="15" width="31.5546875" style="12" customWidth="1"/>
-    <col min="16" max="16" width="25.77734375" style="10" customWidth="1"/>
-    <col min="17" max="17" width="9.21875" style="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.6640625" style="10" customWidth="1"/>
+    <col min="17" max="17" width="9.33203125" style="10" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="17" style="10" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.21875" style="10" customWidth="1"/>
-    <col min="20" max="16384" width="9.21875" style="10"/>
+    <col min="19" max="20" width="9.33203125" style="10" customWidth="1"/>
+    <col min="21" max="16384" width="9.33203125" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1783,7 +1735,7 @@
       <c r="N1" s="31"/>
       <c r="O1" s="22"/>
     </row>
-    <row r="2" spans="1:19" s="20" customFormat="1" ht="14.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" s="20" customFormat="1" ht="14.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="30"/>
       <c r="B2" s="21"/>
       <c r="C2" s="22"/>
@@ -1805,80 +1757,78 @@
     </row>
     <row r="4" spans="1:19" s="11" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="34" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="D4" s="35" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="E4" s="94" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="F4" s="88" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="G4" s="24" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="H4" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="88" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="93" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" s="93" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" s="93" t="s">
+        <v>30</v>
+      </c>
+      <c r="M4" s="90" t="s">
+        <v>31</v>
+      </c>
+      <c r="N4" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="I4" s="88" t="s">
-        <v>34</v>
-      </c>
-      <c r="J4" s="93" t="s">
-        <v>14</v>
-      </c>
-      <c r="K4" s="93" t="s">
-        <v>15</v>
-      </c>
-      <c r="L4" s="93" t="s">
-        <v>18</v>
-      </c>
-      <c r="M4" s="90" t="s">
-        <v>19</v>
-      </c>
-      <c r="N4" s="25" t="s">
-        <v>35</v>
-      </c>
       <c r="O4" s="25" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="P4" s="25" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="Q4" s="25" t="s">
         <v>33</v>
       </c>
       <c r="R4" s="25" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="S4" s="25" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="97" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B5" s="82" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C5" s="59"/>
       <c r="D5" s="57">
         <v>1586.45</v>
       </c>
-      <c r="E5" s="38">
-        <v>1</v>
-      </c>
+      <c r="E5" s="38"/>
       <c r="F5" s="89">
         <f>D5*E5</f>
-        <v>1586.45</v>
+        <v>0</v>
       </c>
       <c r="G5" s="42"/>
       <c r="H5" s="42"/>
@@ -1899,17 +1849,15 @@
         <v>14.04</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="C6" s="55"/>
       <c r="D6" s="57">
         <v>428.34</v>
       </c>
-      <c r="E6" s="38">
-        <v>0</v>
-      </c>
+      <c r="E6" s="38"/>
       <c r="F6" s="89">
-        <f t="shared" ref="F6:F11" si="0">D6*E6</f>
+        <f>D6*E6</f>
         <v>0</v>
       </c>
       <c r="G6" s="42"/>
@@ -1931,17 +1879,15 @@
         <v>14.05</v>
       </c>
       <c r="B7" s="27" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="C7" s="55"/>
       <c r="D7" s="57">
         <v>203.19</v>
       </c>
-      <c r="E7" s="38">
-        <v>0</v>
-      </c>
+      <c r="E7" s="38"/>
       <c r="F7" s="89">
-        <f t="shared" si="0"/>
+        <f>D7*E7</f>
         <v>0</v>
       </c>
       <c r="G7" s="42"/>
@@ -1963,7 +1909,7 @@
         <v>2.14</v>
       </c>
       <c r="B8" s="58" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="C8" s="55"/>
       <c r="D8" s="95">
@@ -1993,17 +1939,15 @@
         <v>3.01</v>
       </c>
       <c r="B9" s="58" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="C9" s="55"/>
       <c r="D9" s="57">
         <v>126.3</v>
       </c>
-      <c r="E9" s="38">
-        <v>0</v>
-      </c>
+      <c r="E9" s="38"/>
       <c r="F9" s="89">
-        <f t="shared" si="0"/>
+        <f>D9*E9</f>
         <v>0</v>
       </c>
       <c r="G9" s="42"/>
@@ -2025,17 +1969,15 @@
         <v>3.02</v>
       </c>
       <c r="B10" s="58" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="C10" s="55"/>
       <c r="D10" s="57">
         <v>203.19</v>
       </c>
-      <c r="E10" s="38">
-        <v>0</v>
-      </c>
+      <c r="E10" s="38"/>
       <c r="F10" s="89">
-        <f t="shared" si="0"/>
+        <f>D10*E10</f>
         <v>0</v>
       </c>
       <c r="G10" s="42"/>
@@ -2057,17 +1999,15 @@
         <v>3.08</v>
       </c>
       <c r="B11" s="58" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="C11" s="55"/>
       <c r="D11" s="57">
         <v>727.07</v>
       </c>
-      <c r="E11" s="38">
-        <v>0</v>
-      </c>
+      <c r="E11" s="38"/>
       <c r="F11" s="89">
-        <f t="shared" si="0"/>
+        <f>D11*E11</f>
         <v>0</v>
       </c>
       <c r="G11" s="42"/>
@@ -9586,10 +9526,10 @@
         <v>17.03</v>
       </c>
       <c r="B369" s="58" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C369" s="55" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="D369" s="57">
         <v>0</v>
@@ -9598,28 +9538,28 @@
         <v>0</v>
       </c>
       <c r="F369" s="89">
-        <f t="shared" ref="F369:F371" si="1">E369*D369</f>
+        <f>E369*D369</f>
         <v>0</v>
       </c>
       <c r="G369" s="42"/>
       <c r="H369" s="42"/>
       <c r="I369" s="89"/>
       <c r="J369" s="55" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="K369" s="57">
         <v>0</v>
       </c>
       <c r="L369" s="38"/>
       <c r="M369" s="89">
-        <f t="shared" ref="M369:M371" si="2">L369*K369</f>
+        <f>L369*K369</f>
         <v>0</v>
       </c>
       <c r="N369" s="42"/>
       <c r="O369" s="50"/>
       <c r="P369" s="51"/>
       <c r="Q369" s="50" t="b">
-        <f t="shared" ref="Q369:Q371" si="3">F369=M369</f>
+        <f>F369=M369</f>
         <v>1</v>
       </c>
       <c r="R369" s="54"/>
@@ -9630,10 +9570,10 @@
         <v>17.04</v>
       </c>
       <c r="B370" s="58" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C370" s="55" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="D370" s="57">
         <v>0</v>
@@ -9642,28 +9582,28 @@
         <v>0</v>
       </c>
       <c r="F370" s="89">
-        <f t="shared" si="1"/>
+        <f>E370*D370</f>
         <v>0</v>
       </c>
       <c r="G370" s="42"/>
       <c r="H370" s="42"/>
       <c r="I370" s="89"/>
       <c r="J370" s="55" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="K370" s="57">
         <v>0</v>
       </c>
       <c r="L370" s="38"/>
       <c r="M370" s="89">
-        <f t="shared" si="2"/>
+        <f>L370*K370</f>
         <v>0</v>
       </c>
       <c r="N370" s="42"/>
       <c r="O370" s="50"/>
       <c r="P370" s="51"/>
       <c r="Q370" s="50" t="b">
-        <f t="shared" si="3"/>
+        <f>F370=M370</f>
         <v>1</v>
       </c>
       <c r="R370" s="54"/>
@@ -9674,10 +9614,10 @@
         <v>17.05</v>
       </c>
       <c r="B371" s="58" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C371" s="55" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="D371" s="57">
         <v>0</v>
@@ -9686,28 +9626,28 @@
         <v>0</v>
       </c>
       <c r="F371" s="89">
-        <f t="shared" si="1"/>
+        <f>E371*D371</f>
         <v>0</v>
       </c>
       <c r="G371" s="42"/>
       <c r="H371" s="42"/>
       <c r="I371" s="89"/>
       <c r="J371" s="55" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="K371" s="57">
         <v>0</v>
       </c>
       <c r="L371" s="38"/>
       <c r="M371" s="89">
-        <f t="shared" si="2"/>
+        <f>L371*K371</f>
         <v>0</v>
       </c>
       <c r="N371" s="42"/>
       <c r="O371" s="50"/>
       <c r="P371" s="51"/>
       <c r="Q371" s="50" t="b">
-        <f t="shared" si="3"/>
+        <f>F371=M371</f>
         <v>1</v>
       </c>
       <c r="R371" s="54"/>
@@ -9716,7 +9656,7 @@
     <row r="372" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A372" s="85"/>
       <c r="B372" s="11" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="M372" s="89">
         <f>L372*F372</f>
@@ -14878,7 +14818,7 @@
       <c r="A2090" s="85"/>
     </row>
   </sheetData>
-  <autoFilter ref="B4:O372" xr:uid="{F49B5569-EF7E-435B-80A6-48F9B475B597}"/>
+  <autoFilter ref="B4:O372" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <conditionalFormatting sqref="A5:A366">
     <cfRule type="duplicateValues" dxfId="2" priority="5"/>
   </conditionalFormatting>
@@ -14891,280 +14831,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003AB5751ECABA6749998EF74675425B7B" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="70ed28ac003b6d379fa35ade6abc2863">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="39a94dcf-b6e2-4f89-b70c-f1c9b6ab0e61" xmlns:ns4="62ff2926-d3aa-4d63-a80f-1987d6b279cc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7e138214fb60f7ac65bb94e3793bb0af" ns3:_="" ns4:_="">
-    <xsd:import namespace="39a94dcf-b6e2-4f89-b70c-f1c9b6ab0e61"/>
-    <xsd:import namespace="62ff2926-d3aa-4d63-a80f-1987d6b279cc"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceAutoTags" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceLocation" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns4:SharedWithUsers" minOccurs="0"/>
-                <xsd:element ref="ns4:SharedWithDetails" minOccurs="0"/>
-                <xsd:element ref="ns4:SharingHintHash" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceAutoKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns3:MediaServiceKeyPoints" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="39a94dcf-b6e2-4f89-b70c-f1c9b6ab0e61" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoTags" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoTags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="11" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="12" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceLocation" ma:index="13" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="14" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="15" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="19" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceKeyPoints" ma:index="20" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="62ff2926-d3aa-4d63-a80f-1987d6b279cc" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="16" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:UserMulti">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="17" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="SharingHintHash" ma:index="18" nillable="true" ma:displayName="Sharing Hint Hash" ma:hidden="true" ma:internalName="SharingHintHash" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2921983E-6AF9-412A-AD58-3980A2719A16}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F138C2C4-D118-4DE3-AAEA-5BBC3FF040F7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E7C5A98-C3A1-4BF8-8017-645861449BF9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="39a94dcf-b6e2-4f89-b70c-f1c9b6ab0e61"/>
-    <ds:schemaRef ds:uri="62ff2926-d3aa-4d63-a80f-1987d6b279cc"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>